<commit_message>
fix: replace deprecated experimental_rerun with st.rerun and ensure classifications save correctly
</commit_message>
<xml_diff>
--- a/Modelo_Extrato_Vledger.xlsx
+++ b/Modelo_Extrato_Vledger.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sn1102006\Desktop\projetos\Vledger\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1700B0-AE0E-4381-8657-513EC0111ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>DATA</t>
   </si>
@@ -35,15 +41,6 @@
   </si>
   <si>
     <t>NF</t>
-  </si>
-  <si>
-    <t>05/10/2025</t>
-  </si>
-  <si>
-    <t>06/10/2025</t>
-  </si>
-  <si>
-    <t>07/10/2025</t>
   </si>
   <si>
     <t>INTERMEDICA</t>
@@ -67,8 +64,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,24 +117,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -175,7 +181,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -209,6 +215,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -243,9 +250,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -418,14 +426,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -448,67 +461,67 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>45874</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>45875</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>45876</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>45876</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
       </c>
       <c r="C5">
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>9</v>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>45876</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C6">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>9</v>
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>45876</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <v>568</v>

</xml_diff>